<commit_message>
Completed LO 3-2 - compare at least three techniques for improving team effectiveness
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED88E3D9-ECC0-7241-8CEE-3C6A98C6761D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382386B8-8714-C245-B87E-9AFF6322DB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23740" yWindow="5920" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="230">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -1712,6 +1712,12 @@
   <si>
     <t>Total Self- Learning (Hrs)</t>
   </si>
+  <si>
+    <t>4/16/24</t>
+  </si>
+  <si>
+    <t>Deep dive on LO 3.2 - Improving teams effectiveness</t>
+  </si>
 </sst>
 </file>
 
@@ -2466,30 +2472,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2503,30 +2516,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16905,18 +16911,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="72"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="98"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17037,13 +17043,13 @@
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="73">
+      <c r="B6" s="94">
         <v>1</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="85" t="s">
         <v>124</v>
       </c>
       <c r="E6" s="49" t="s">
@@ -17077,9 +17083,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="24"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="49" t="s">
         <v>127</v>
       </c>
@@ -17110,9 +17116,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="49" t="s">
         <v>129</v>
       </c>
@@ -17144,9 +17150,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="74"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="49" t="s">
         <v>131</v>
       </c>
@@ -17181,10 +17187,10 @@
       <c r="B10" s="80">
         <v>2</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="85" t="s">
         <v>134</v>
       </c>
       <c r="E10" s="49" t="s">
@@ -17218,9 +17224,9 @@
     </row>
     <row r="11" spans="1:28" ht="49.5" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="49" t="s">
         <v>137</v>
       </c>
@@ -17252,9 +17258,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="49" t="s">
         <v>139</v>
       </c>
@@ -17286,9 +17292,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="75"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="49" t="s">
         <v>141</v>
       </c>
@@ -17320,9 +17326,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="79" t="s">
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="93" t="s">
         <v>143</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -17356,9 +17362,9 @@
     </row>
     <row r="15" spans="1:28" ht="49.5" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
       <c r="E15" s="49" t="s">
         <v>146</v>
       </c>
@@ -17390,9 +17396,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="49" t="s">
         <v>148</v>
       </c>
@@ -17424,9 +17430,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="49" t="s">
         <v>150</v>
       </c>
@@ -17458,13 +17464,13 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="73">
+      <c r="B18" s="94">
         <v>3</v>
       </c>
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="79" t="s">
+      <c r="D18" s="93" t="s">
         <v>153</v>
       </c>
       <c r="E18" s="49" t="s">
@@ -17498,9 +17504,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="75"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
@@ -17532,9 +17538,9 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="77" t="s">
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="85" t="s">
         <v>158</v>
       </c>
       <c r="E20" s="56" t="s">
@@ -17568,9 +17574,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
       <c r="E21" s="49" t="s">
         <v>161</v>
       </c>
@@ -17602,9 +17608,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
       <c r="E22" s="49" t="s">
         <v>163</v>
       </c>
@@ -17636,9 +17642,9 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="75"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="49" t="s">
         <v>165</v>
       </c>
@@ -17670,13 +17676,13 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="73">
+      <c r="B24" s="94">
         <v>4</v>
       </c>
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="95" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="79" t="s">
+      <c r="D24" s="93" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -17710,9 +17716,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="49" t="s">
         <v>171</v>
       </c>
@@ -17747,10 +17753,10 @@
       <c r="B26" s="80">
         <v>5</v>
       </c>
-      <c r="C26" s="78" t="s">
+      <c r="C26" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="79" t="s">
+      <c r="D26" s="93" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="49" t="s">
@@ -17784,9 +17790,9 @@
     </row>
     <row r="27" spans="1:28" ht="49.5" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
       <c r="E27" s="49" t="s">
         <v>177</v>
       </c>
@@ -17818,9 +17824,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
       <c r="E28" s="49" t="s">
         <v>179</v>
       </c>
@@ -17852,9 +17858,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="49" t="s">
         <v>181</v>
       </c>
@@ -17886,9 +17892,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="79" t="s">
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="93" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="49" t="s">
@@ -17922,9 +17928,9 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
       <c r="E31" s="49" t="s">
         <v>186</v>
       </c>
@@ -17956,9 +17962,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
       <c r="E32" s="49" t="s">
         <v>188</v>
       </c>
@@ -17993,10 +17999,10 @@
       <c r="B33" s="80">
         <v>6</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C33" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="79" t="s">
+      <c r="D33" s="93" t="s">
         <v>191</v>
       </c>
       <c r="E33" s="49" t="s">
@@ -18030,9 +18036,9 @@
     </row>
     <row r="34" spans="1:28" ht="49.5" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
       <c r="E34" s="58" t="s">
         <v>194</v>
       </c>
@@ -18063,36 +18069,36 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="87"/>
-      <c r="B35" s="87" t="s">
+      <c r="A35" s="82"/>
+      <c r="B35" s="82" t="s">
         <v>196</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="84" t="s">
         <v>197</v>
       </c>
-      <c r="D35" s="77" t="s">
+      <c r="D35" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="89" t="s">
+      <c r="E35" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="87" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="81" t="s">
+      <c r="G35" s="88" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="82" t="s">
+      <c r="H35" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="83">
+      <c r="I35" s="90">
         <v>45389</v>
       </c>
-      <c r="J35" s="84" t="s">
+      <c r="J35" s="91" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="82"/>
-      <c r="L35" s="85"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="78"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -18111,18 +18117,18 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="86"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="79"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -18141,18 +18147,18 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
-      <c r="B37" s="74"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="74"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="86"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="79"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -18171,18 +18177,18 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="74"/>
-      <c r="B38" s="74"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="86"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="83"/>
+      <c r="J38" s="83"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="79"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -18201,18 +18207,18 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="74"/>
-      <c r="B39" s="74"/>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="74"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="74"/>
-      <c r="L39" s="86"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="79"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -18231,18 +18237,18 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="75"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
-      <c r="L40" s="86"/>
+      <c r="A40" s="81"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="81"/>
+      <c r="L40" s="79"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -24877,6 +24883,27 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="L35:L40"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A40"/>
@@ -24890,27 +24917,6 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="J35:J40"/>
     <mergeCell ref="K35:K40"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -31690,7 +31696,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31739,20 +31745,20 @@
       <c r="Z1" s="15"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="92">
+      <c r="A2" s="71">
         <v>45385</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="72" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="93">
+      <c r="D2" s="72">
         <v>1</v>
       </c>
       <c r="E2" s="15"/>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="70" t="s">
         <v>227</v>
       </c>
       <c r="G2" s="15"/>
@@ -31777,22 +31783,22 @@
       <c r="Z2" s="15"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="95">
+      <c r="A3" s="74">
         <v>45387</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="75" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="D3" s="96">
+      <c r="D3" s="75">
         <v>2</v>
       </c>
       <c r="E3" s="15"/>
-      <c r="F3" s="91">
+      <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -31816,16 +31822,16 @@
       <c r="Z3" s="15"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="97">
+      <c r="A4" s="76">
         <v>45539</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="77" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="98">
+      <c r="D4" s="77">
         <v>2</v>
       </c>
       <c r="E4" s="15"/>
@@ -31852,16 +31858,16 @@
       <c r="Z4" s="15"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="97">
+      <c r="A5" s="76">
         <v>45569</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="77" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="98">
+      <c r="D5" s="77">
         <v>1</v>
       </c>
       <c r="E5" s="15"/>
@@ -31888,16 +31894,16 @@
       <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="97">
+      <c r="A6" s="76">
         <v>45630</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="77" t="s">
         <v>222</v>
       </c>
-      <c r="D6" s="98">
+      <c r="D6" s="77">
         <v>3.5</v>
       </c>
       <c r="E6" s="15"/>
@@ -31924,16 +31930,16 @@
       <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="77" t="s">
         <v>223</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="77" t="s">
         <v>224</v>
       </c>
-      <c r="D7" s="98">
+      <c r="D7" s="77">
         <v>1</v>
       </c>
       <c r="E7" s="15"/>
@@ -31960,16 +31966,16 @@
       <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="77" t="s">
         <v>225</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="98" t="s">
+      <c r="C8" s="77" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="98">
+      <c r="D8" s="77">
         <v>2</v>
       </c>
       <c r="E8" s="15"/>
@@ -31996,10 +32002,18 @@
       <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="96"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
+      <c r="A9" s="75" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>229</v>
+      </c>
+      <c r="D9" s="75">
+        <v>1</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -32024,10 +32038,10 @@
       <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="94"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>

</xml_diff>

<commit_message>
Updated LO 2-5 create a coaching agreement with an individual or a team
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382386B8-8714-C245-B87E-9AFF6322DB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DB28C-9A24-C649-8C82-C43C6F4F8994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23740" yWindow="5920" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="1" r:id="rId1"/>
@@ -2480,23 +2480,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2516,23 +2533,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16911,18 +16911,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="80"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17043,10 +17043,10 @@
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="94">
+      <c r="B6" s="81">
         <v>1</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="84" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="85" t="s">
@@ -17083,9 +17083,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="24"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="49" t="s">
         <v>127</v>
       </c>
@@ -17116,9 +17116,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="49" t="s">
         <v>129</v>
       </c>
@@ -17150,9 +17150,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="83"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="49" t="s">
         <v>131</v>
       </c>
@@ -17184,10 +17184,10 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="24"/>
-      <c r="B10" s="80">
+      <c r="B10" s="88">
         <v>2</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="86" t="s">
         <v>133</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -17224,9 +17224,9 @@
     </row>
     <row r="11" spans="1:28" ht="49.5" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="49" t="s">
         <v>137</v>
       </c>
@@ -17258,9 +17258,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
       <c r="E12" s="49" t="s">
         <v>139</v>
       </c>
@@ -17292,9 +17292,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="81"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="49" t="s">
         <v>141</v>
       </c>
@@ -17326,9 +17326,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="93" t="s">
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="87" t="s">
         <v>143</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -17362,9 +17362,9 @@
     </row>
     <row r="15" spans="1:28" ht="49.5" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
       <c r="E15" s="49" t="s">
         <v>146</v>
       </c>
@@ -17396,9 +17396,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
       <c r="E16" s="49" t="s">
         <v>148</v>
       </c>
@@ -17430,9 +17430,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="49" t="s">
         <v>150</v>
       </c>
@@ -17464,13 +17464,13 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="94">
+      <c r="B18" s="81">
         <v>3</v>
       </c>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="87" t="s">
         <v>153</v>
       </c>
       <c r="E18" s="49" t="s">
@@ -17504,9 +17504,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="81"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
@@ -17538,8 +17538,8 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="85" t="s">
         <v>158</v>
       </c>
@@ -17574,9 +17574,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="49" t="s">
         <v>161</v>
       </c>
@@ -17608,9 +17608,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="49" t="s">
         <v>163</v>
       </c>
@@ -17642,9 +17642,9 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
       <c r="E23" s="49" t="s">
         <v>165</v>
       </c>
@@ -17676,13 +17676,13 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="94">
+      <c r="B24" s="81">
         <v>4</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="93" t="s">
+      <c r="D24" s="87" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -17716,9 +17716,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
       <c r="E25" s="49" t="s">
         <v>171</v>
       </c>
@@ -17750,13 +17750,13 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="24"/>
-      <c r="B26" s="80">
+      <c r="B26" s="88">
         <v>5</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="93" t="s">
+      <c r="D26" s="87" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="49" t="s">
@@ -17790,9 +17790,9 @@
     </row>
     <row r="27" spans="1:28" ht="49.5" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="49" t="s">
         <v>177</v>
       </c>
@@ -17824,9 +17824,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="49" t="s">
         <v>179</v>
       </c>
@@ -17858,9 +17858,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="81"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="83"/>
       <c r="E29" s="49" t="s">
         <v>181</v>
       </c>
@@ -17892,9 +17892,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="93" t="s">
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="49" t="s">
@@ -17928,9 +17928,9 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
       <c r="E31" s="49" t="s">
         <v>186</v>
       </c>
@@ -17962,9 +17962,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
       <c r="E32" s="49" t="s">
         <v>188</v>
       </c>
@@ -17996,13 +17996,13 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="24"/>
-      <c r="B33" s="80">
+      <c r="B33" s="88">
         <v>6</v>
       </c>
-      <c r="C33" s="92" t="s">
+      <c r="C33" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="93" t="s">
+      <c r="D33" s="87" t="s">
         <v>191</v>
       </c>
       <c r="E33" s="49" t="s">
@@ -18036,9 +18036,9 @@
     </row>
     <row r="34" spans="1:28" ht="49.5" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
       <c r="E34" s="58" t="s">
         <v>194</v>
       </c>
@@ -18069,36 +18069,36 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="82"/>
-      <c r="B35" s="82" t="s">
+      <c r="A35" s="91"/>
+      <c r="B35" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="92" t="s">
         <v>197</v>
       </c>
       <c r="D35" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="86" t="s">
+      <c r="E35" s="93" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="87" t="s">
+      <c r="F35" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="88" t="s">
+      <c r="G35" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="89" t="s">
+      <c r="H35" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="90">
+      <c r="I35" s="97">
         <v>45389</v>
       </c>
-      <c r="J35" s="91" t="s">
+      <c r="J35" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="89"/>
-      <c r="L35" s="78"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="89"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -18117,18 +18117,18 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="83"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="79"/>
+      <c r="A36" s="82"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="90"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -18147,18 +18147,18 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="83"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="79"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="90"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -18177,18 +18177,18 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="83"/>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="79"/>
+      <c r="A38" s="82"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="90"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -18207,18 +18207,18 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="83"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
-      <c r="J39" s="83"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="79"/>
+      <c r="A39" s="82"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="90"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -18237,18 +18237,18 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="81"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="79"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="83"/>
+      <c r="K40" s="83"/>
+      <c r="L40" s="90"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -24883,27 +24883,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
     <mergeCell ref="L35:L40"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A40"/>
@@ -24917,6 +24896,27 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="J35:J40"/>
     <mergeCell ref="K35:K40"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -31696,7 +31696,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31798,7 +31798,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>13.5</v>
+        <v>14</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32012,7 +32012,7 @@
         <v>229</v>
       </c>
       <c r="D9" s="75">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>

</xml_diff>

<commit_message>
Completed LO 3-4 - plan the launch of a new Scrum Team
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DB28C-9A24-C649-8C82-C43C6F4F8994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32796AA7-43ED-484F-943E-B2E845D23EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1716,7 +1716,7 @@
     <t>4/16/24</t>
   </si>
   <si>
-    <t>Deep dive on LO 3.2 - Improving teams effectiveness</t>
+    <t>Deep dive on LO 3.2 - 3.4</t>
   </si>
 </sst>
 </file>
@@ -2480,40 +2480,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2533,6 +2516,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16911,18 +16911,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="80"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="98"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17043,10 +17043,10 @@
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="81">
+      <c r="B6" s="94">
         <v>1</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="95" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="85" t="s">
@@ -17083,9 +17083,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="24"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="49" t="s">
         <v>127</v>
       </c>
@@ -17116,9 +17116,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="49" t="s">
         <v>129</v>
       </c>
@@ -17150,9 +17150,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="49" t="s">
         <v>131</v>
       </c>
@@ -17184,10 +17184,10 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="24"/>
-      <c r="B10" s="88">
+      <c r="B10" s="80">
         <v>2</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="92" t="s">
         <v>133</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -17224,9 +17224,9 @@
     </row>
     <row r="11" spans="1:28" ht="49.5" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="49" t="s">
         <v>137</v>
       </c>
@@ -17258,9 +17258,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="49" t="s">
         <v>139</v>
       </c>
@@ -17292,9 +17292,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="49" t="s">
         <v>141</v>
       </c>
@@ -17326,9 +17326,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="87" t="s">
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="93" t="s">
         <v>143</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -17362,9 +17362,9 @@
     </row>
     <row r="15" spans="1:28" ht="49.5" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
       <c r="E15" s="49" t="s">
         <v>146</v>
       </c>
@@ -17396,9 +17396,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="49" t="s">
         <v>148</v>
       </c>
@@ -17430,9 +17430,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="49" t="s">
         <v>150</v>
       </c>
@@ -17464,13 +17464,13 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="81">
+      <c r="B18" s="94">
         <v>3</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="93" t="s">
         <v>153</v>
       </c>
       <c r="E18" s="49" t="s">
@@ -17504,9 +17504,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="83"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
@@ -17538,8 +17538,8 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="85" t="s">
         <v>158</v>
       </c>
@@ -17574,9 +17574,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
       <c r="E21" s="49" t="s">
         <v>161</v>
       </c>
@@ -17608,9 +17608,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
       <c r="E22" s="49" t="s">
         <v>163</v>
       </c>
@@ -17642,9 +17642,9 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="49" t="s">
         <v>165</v>
       </c>
@@ -17676,13 +17676,13 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="81">
+      <c r="B24" s="94">
         <v>4</v>
       </c>
-      <c r="C24" s="84" t="s">
+      <c r="C24" s="95" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="87" t="s">
+      <c r="D24" s="93" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -17716,9 +17716,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="49" t="s">
         <v>171</v>
       </c>
@@ -17750,13 +17750,13 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="24"/>
-      <c r="B26" s="88">
+      <c r="B26" s="80">
         <v>5</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="93" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="49" t="s">
@@ -17790,9 +17790,9 @@
     </row>
     <row r="27" spans="1:28" ht="49.5" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
       <c r="E27" s="49" t="s">
         <v>177</v>
       </c>
@@ -17824,9 +17824,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
       <c r="E28" s="49" t="s">
         <v>179</v>
       </c>
@@ -17858,9 +17858,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="83"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="49" t="s">
         <v>181</v>
       </c>
@@ -17892,9 +17892,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="87" t="s">
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="93" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="49" t="s">
@@ -17928,9 +17928,9 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
       <c r="E31" s="49" t="s">
         <v>186</v>
       </c>
@@ -17962,9 +17962,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
       <c r="E32" s="49" t="s">
         <v>188</v>
       </c>
@@ -17996,13 +17996,13 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="24"/>
-      <c r="B33" s="88">
+      <c r="B33" s="80">
         <v>6</v>
       </c>
-      <c r="C33" s="86" t="s">
+      <c r="C33" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="93" t="s">
         <v>191</v>
       </c>
       <c r="E33" s="49" t="s">
@@ -18036,9 +18036,9 @@
     </row>
     <row r="34" spans="1:28" ht="49.5" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
       <c r="E34" s="58" t="s">
         <v>194</v>
       </c>
@@ -18069,36 +18069,36 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="91"/>
-      <c r="B35" s="91" t="s">
+      <c r="A35" s="82"/>
+      <c r="B35" s="82" t="s">
         <v>196</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="84" t="s">
         <v>197</v>
       </c>
       <c r="D35" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="93" t="s">
+      <c r="E35" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="94" t="s">
+      <c r="F35" s="87" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="95" t="s">
+      <c r="G35" s="88" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="96" t="s">
+      <c r="H35" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="97">
+      <c r="I35" s="90">
         <v>45389</v>
       </c>
-      <c r="J35" s="98" t="s">
+      <c r="J35" s="91" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="96"/>
-      <c r="L35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="78"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -18117,18 +18117,18 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="82"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="82"/>
-      <c r="L36" s="90"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="79"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -18147,18 +18147,18 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="82"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="82"/>
-      <c r="L37" s="90"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="79"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -18177,18 +18177,18 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="82"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="82"/>
-      <c r="J38" s="82"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="90"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="83"/>
+      <c r="J38" s="83"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="79"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -18207,18 +18207,18 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="82"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="90"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="79"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -18237,18 +18237,18 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="83"/>
-      <c r="B40" s="83"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="83"/>
-      <c r="K40" s="83"/>
-      <c r="L40" s="90"/>
+      <c r="A40" s="81"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="81"/>
+      <c r="L40" s="79"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -24883,6 +24883,27 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="L35:L40"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A40"/>
@@ -24896,27 +24917,6 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="J35:J40"/>
     <mergeCell ref="K35:K40"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -31696,7 +31696,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31798,7 +31798,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>14</v>
+        <v>15.5</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32012,7 +32012,7 @@
         <v>229</v>
       </c>
       <c r="D9" s="75">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>

</xml_diff>

<commit_message>
Completed LO 3-6 - illustrate how at least one element of software craftsmanship applies to your work
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32796AA7-43ED-484F-943E-B2E845D23EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84230981-3F02-984E-981E-A3689521AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="231">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -1718,6 +1718,9 @@
   <si>
     <t>Deep dive on LO 3.2 - 3.4</t>
   </si>
+  <si>
+    <t>Deep dive L0 3.5 -3.6</t>
+  </si>
 </sst>
 </file>
 
@@ -2480,23 +2483,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2516,23 +2536,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16911,18 +16914,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="80"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17043,10 +17046,10 @@
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="94">
+      <c r="B6" s="81">
         <v>1</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="84" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="85" t="s">
@@ -17083,9 +17086,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="24"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="49" t="s">
         <v>127</v>
       </c>
@@ -17116,9 +17119,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="49" t="s">
         <v>129</v>
       </c>
@@ -17150,9 +17153,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="83"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="49" t="s">
         <v>131</v>
       </c>
@@ -17184,10 +17187,10 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="24"/>
-      <c r="B10" s="80">
+      <c r="B10" s="88">
         <v>2</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="86" t="s">
         <v>133</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -17224,9 +17227,9 @@
     </row>
     <row r="11" spans="1:28" ht="49.5" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="49" t="s">
         <v>137</v>
       </c>
@@ -17258,9 +17261,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
       <c r="E12" s="49" t="s">
         <v>139</v>
       </c>
@@ -17292,9 +17295,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="81"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="49" t="s">
         <v>141</v>
       </c>
@@ -17326,9 +17329,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="93" t="s">
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="87" t="s">
         <v>143</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -17362,9 +17365,9 @@
     </row>
     <row r="15" spans="1:28" ht="49.5" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
       <c r="E15" s="49" t="s">
         <v>146</v>
       </c>
@@ -17396,9 +17399,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
       <c r="E16" s="49" t="s">
         <v>148</v>
       </c>
@@ -17430,9 +17433,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="49" t="s">
         <v>150</v>
       </c>
@@ -17464,13 +17467,13 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="94">
+      <c r="B18" s="81">
         <v>3</v>
       </c>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="87" t="s">
         <v>153</v>
       </c>
       <c r="E18" s="49" t="s">
@@ -17504,9 +17507,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="81"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
@@ -17538,8 +17541,8 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="85" t="s">
         <v>158</v>
       </c>
@@ -17574,9 +17577,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="49" t="s">
         <v>161</v>
       </c>
@@ -17608,9 +17611,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="49" t="s">
         <v>163</v>
       </c>
@@ -17642,9 +17645,9 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
       <c r="E23" s="49" t="s">
         <v>165</v>
       </c>
@@ -17676,13 +17679,13 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="94">
+      <c r="B24" s="81">
         <v>4</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="93" t="s">
+      <c r="D24" s="87" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -17716,9 +17719,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
       <c r="E25" s="49" t="s">
         <v>171</v>
       </c>
@@ -17750,13 +17753,13 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="24"/>
-      <c r="B26" s="80">
+      <c r="B26" s="88">
         <v>5</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="93" t="s">
+      <c r="D26" s="87" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="49" t="s">
@@ -17790,9 +17793,9 @@
     </row>
     <row r="27" spans="1:28" ht="49.5" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="49" t="s">
         <v>177</v>
       </c>
@@ -17824,9 +17827,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="49" t="s">
         <v>179</v>
       </c>
@@ -17858,9 +17861,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="81"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="83"/>
       <c r="E29" s="49" t="s">
         <v>181</v>
       </c>
@@ -17892,9 +17895,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="93" t="s">
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="49" t="s">
@@ -17928,9 +17931,9 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
       <c r="E31" s="49" t="s">
         <v>186</v>
       </c>
@@ -17962,9 +17965,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
       <c r="E32" s="49" t="s">
         <v>188</v>
       </c>
@@ -17996,13 +17999,13 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="24"/>
-      <c r="B33" s="80">
+      <c r="B33" s="88">
         <v>6</v>
       </c>
-      <c r="C33" s="92" t="s">
+      <c r="C33" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="93" t="s">
+      <c r="D33" s="87" t="s">
         <v>191</v>
       </c>
       <c r="E33" s="49" t="s">
@@ -18036,9 +18039,9 @@
     </row>
     <row r="34" spans="1:28" ht="49.5" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
       <c r="E34" s="58" t="s">
         <v>194</v>
       </c>
@@ -18069,36 +18072,36 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="82"/>
-      <c r="B35" s="82" t="s">
+      <c r="A35" s="91"/>
+      <c r="B35" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="92" t="s">
         <v>197</v>
       </c>
       <c r="D35" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="86" t="s">
+      <c r="E35" s="93" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="87" t="s">
+      <c r="F35" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="88" t="s">
+      <c r="G35" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="89" t="s">
+      <c r="H35" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="90">
+      <c r="I35" s="97">
         <v>45389</v>
       </c>
-      <c r="J35" s="91" t="s">
+      <c r="J35" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="89"/>
-      <c r="L35" s="78"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="89"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -18117,18 +18120,18 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="83"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="79"/>
+      <c r="A36" s="82"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="90"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -18147,18 +18150,18 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="83"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="79"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="90"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -18177,18 +18180,18 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="83"/>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="79"/>
+      <c r="A38" s="82"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="90"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -18207,18 +18210,18 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="83"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
-      <c r="J39" s="83"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="79"/>
+      <c r="A39" s="82"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="90"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -18237,18 +18240,18 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="81"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="79"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="83"/>
+      <c r="K40" s="83"/>
+      <c r="L40" s="90"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -24883,27 +24886,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
     <mergeCell ref="L35:L40"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A40"/>
@@ -24917,6 +24899,27 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="J35:J40"/>
     <mergeCell ref="K35:K40"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -31696,7 +31699,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31798,7 +31801,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>15.5</v>
+        <v>17</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32038,10 +32041,18 @@
       <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
+      <c r="A10" s="75" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="73">
+        <v>1.5</v>
+      </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>

</xml_diff>

<commit_message>
Completed LO 4.1 - 1 - Mind Map
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84230981-3F02-984E-981E-A3689521AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22541B8C-D2A8-FA47-BD53-AEF9D34BEE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="233">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -1721,6 +1721,12 @@
   <si>
     <t>Deep dive L0 3.5 -3.6</t>
   </si>
+  <si>
+    <t>Deep dive - LO 4.1</t>
+  </si>
+  <si>
+    <t>4/18/24</t>
+  </si>
 </sst>
 </file>
 
@@ -2483,40 +2489,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2536,6 +2525,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16914,18 +16920,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="80"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="98"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17046,10 +17052,10 @@
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="81">
+      <c r="B6" s="94">
         <v>1</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="95" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="85" t="s">
@@ -17086,9 +17092,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="24"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="49" t="s">
         <v>127</v>
       </c>
@@ -17119,9 +17125,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="49" t="s">
         <v>129</v>
       </c>
@@ -17153,9 +17159,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="83"/>
       <c r="E9" s="49" t="s">
         <v>131</v>
       </c>
@@ -17187,10 +17193,10 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="24"/>
-      <c r="B10" s="88">
+      <c r="B10" s="80">
         <v>2</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="92" t="s">
         <v>133</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -17227,9 +17233,9 @@
     </row>
     <row r="11" spans="1:28" ht="49.5" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
       <c r="E11" s="49" t="s">
         <v>137</v>
       </c>
@@ -17261,9 +17267,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
       <c r="E12" s="49" t="s">
         <v>139</v>
       </c>
@@ -17295,9 +17301,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="49" t="s">
         <v>141</v>
       </c>
@@ -17329,9 +17335,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="87" t="s">
+      <c r="B14" s="83"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="93" t="s">
         <v>143</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -17365,9 +17371,9 @@
     </row>
     <row r="15" spans="1:28" ht="49.5" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
       <c r="E15" s="49" t="s">
         <v>146</v>
       </c>
@@ -17399,9 +17405,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="82"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="83"/>
       <c r="E16" s="49" t="s">
         <v>148</v>
       </c>
@@ -17433,9 +17439,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="49" t="s">
         <v>150</v>
       </c>
@@ -17467,13 +17473,13 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="81">
+      <c r="B18" s="94">
         <v>3</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="92" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="87" t="s">
+      <c r="D18" s="93" t="s">
         <v>153</v>
       </c>
       <c r="E18" s="49" t="s">
@@ -17507,9 +17513,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="83"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
@@ -17541,8 +17547,8 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="82"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="85" t="s">
         <v>158</v>
       </c>
@@ -17577,9 +17583,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
       <c r="E21" s="49" t="s">
         <v>161</v>
       </c>
@@ -17611,9 +17617,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
       <c r="E22" s="49" t="s">
         <v>163</v>
       </c>
@@ -17645,9 +17651,9 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="49" t="s">
         <v>165</v>
       </c>
@@ -17679,13 +17685,13 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="81">
+      <c r="B24" s="94">
         <v>4</v>
       </c>
-      <c r="C24" s="84" t="s">
+      <c r="C24" s="95" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="87" t="s">
+      <c r="D24" s="93" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -17719,9 +17725,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="83"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="49" t="s">
         <v>171</v>
       </c>
@@ -17753,13 +17759,13 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="24"/>
-      <c r="B26" s="88">
+      <c r="B26" s="80">
         <v>5</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="87" t="s">
+      <c r="D26" s="93" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="49" t="s">
@@ -17793,9 +17799,9 @@
     </row>
     <row r="27" spans="1:28" ht="49.5" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
       <c r="E27" s="49" t="s">
         <v>177</v>
       </c>
@@ -17827,9 +17833,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
       <c r="E28" s="49" t="s">
         <v>179</v>
       </c>
@@ -17861,9 +17867,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="83"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="49" t="s">
         <v>181</v>
       </c>
@@ -17895,9 +17901,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="82"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="87" t="s">
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="93" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="49" t="s">
@@ -17931,9 +17937,9 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
       <c r="E31" s="49" t="s">
         <v>186</v>
       </c>
@@ -17965,9 +17971,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="83"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
       <c r="E32" s="49" t="s">
         <v>188</v>
       </c>
@@ -17999,13 +18005,13 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="24"/>
-      <c r="B33" s="88">
+      <c r="B33" s="80">
         <v>6</v>
       </c>
-      <c r="C33" s="86" t="s">
+      <c r="C33" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="87" t="s">
+      <c r="D33" s="93" t="s">
         <v>191</v>
       </c>
       <c r="E33" s="49" t="s">
@@ -18039,9 +18045,9 @@
     </row>
     <row r="34" spans="1:28" ht="49.5" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="83"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
       <c r="E34" s="58" t="s">
         <v>194</v>
       </c>
@@ -18072,36 +18078,36 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="91"/>
-      <c r="B35" s="91" t="s">
+      <c r="A35" s="82"/>
+      <c r="B35" s="82" t="s">
         <v>196</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="84" t="s">
         <v>197</v>
       </c>
       <c r="D35" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="93" t="s">
+      <c r="E35" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="94" t="s">
+      <c r="F35" s="87" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="95" t="s">
+      <c r="G35" s="88" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="96" t="s">
+      <c r="H35" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="97">
+      <c r="I35" s="90">
         <v>45389</v>
       </c>
-      <c r="J35" s="98" t="s">
+      <c r="J35" s="91" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="96"/>
-      <c r="L35" s="89"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="78"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -18120,18 +18126,18 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="82"/>
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
-      <c r="E36" s="82"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-      <c r="H36" s="82"/>
-      <c r="I36" s="82"/>
-      <c r="J36" s="82"/>
-      <c r="K36" s="82"/>
-      <c r="L36" s="90"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="79"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -18150,18 +18156,18 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="82"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="82"/>
-      <c r="L37" s="90"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="79"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -18180,18 +18186,18 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="82"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="82"/>
-      <c r="J38" s="82"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="90"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="83"/>
+      <c r="J38" s="83"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="79"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -18210,18 +18216,18 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="82"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="90"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="79"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -18240,18 +18246,18 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="83"/>
-      <c r="B40" s="83"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="83"/>
-      <c r="K40" s="83"/>
-      <c r="L40" s="90"/>
+      <c r="A40" s="81"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="81"/>
+      <c r="E40" s="81"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="81"/>
+      <c r="H40" s="81"/>
+      <c r="I40" s="81"/>
+      <c r="J40" s="81"/>
+      <c r="K40" s="81"/>
+      <c r="L40" s="79"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -24886,6 +24892,27 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="L35:L40"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A40"/>
@@ -24899,27 +24926,6 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="J35:J40"/>
     <mergeCell ref="K35:K40"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -31699,7 +31705,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31801,7 +31807,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32077,10 +32083,18 @@
       <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="75" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>

</xml_diff>

<commit_message>
Completed LO 4.1 apply at least two techniques for moving from Product Goal to Product Backlog
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22541B8C-D2A8-FA47-BD53-AEF9D34BEE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BB2D41-F431-CD46-9D0F-9CF1CFEEE4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2489,23 +2489,40 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="60" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2525,23 +2542,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16920,18 +16920,18 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
       <c r="A3" s="24"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="80"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -17052,10 +17052,10 @@
     </row>
     <row r="6" spans="1:28" ht="49.5" customHeight="1">
       <c r="A6" s="24"/>
-      <c r="B6" s="94">
+      <c r="B6" s="81">
         <v>1</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="84" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="85" t="s">
@@ -17092,9 +17092,9 @@
     </row>
     <row r="7" spans="1:28" ht="49.5" customHeight="1">
       <c r="A7" s="24"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="49" t="s">
         <v>127</v>
       </c>
@@ -17125,9 +17125,9 @@
     </row>
     <row r="8" spans="1:28" ht="49.5" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="49" t="s">
         <v>129</v>
       </c>
@@ -17159,9 +17159,9 @@
     </row>
     <row r="9" spans="1:28" ht="49.5" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="83"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="49" t="s">
         <v>131</v>
       </c>
@@ -17193,10 +17193,10 @@
     </row>
     <row r="10" spans="1:28" ht="49.5" customHeight="1">
       <c r="A10" s="24"/>
-      <c r="B10" s="80">
+      <c r="B10" s="88">
         <v>2</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="86" t="s">
         <v>133</v>
       </c>
       <c r="D10" s="85" t="s">
@@ -17233,9 +17233,9 @@
     </row>
     <row r="11" spans="1:28" ht="49.5" customHeight="1">
       <c r="A11" s="24"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="49" t="s">
         <v>137</v>
       </c>
@@ -17267,9 +17267,9 @@
     </row>
     <row r="12" spans="1:28" ht="49.5" customHeight="1">
       <c r="A12" s="24"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
       <c r="E12" s="49" t="s">
         <v>139</v>
       </c>
@@ -17301,9 +17301,9 @@
     </row>
     <row r="13" spans="1:28" ht="49.5" customHeight="1">
       <c r="A13" s="24"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="81"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83"/>
       <c r="E13" s="49" t="s">
         <v>141</v>
       </c>
@@ -17335,9 +17335,9 @@
     </row>
     <row r="14" spans="1:28" ht="49.5" customHeight="1">
       <c r="A14" s="24"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="93" t="s">
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="87" t="s">
         <v>143</v>
       </c>
       <c r="E14" s="49" t="s">
@@ -17371,9 +17371,9 @@
     </row>
     <row r="15" spans="1:28" ht="49.5" customHeight="1">
       <c r="A15" s="24"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
       <c r="E15" s="49" t="s">
         <v>146</v>
       </c>
@@ -17405,9 +17405,9 @@
     </row>
     <row r="16" spans="1:28" ht="49.5" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
       <c r="E16" s="49" t="s">
         <v>148</v>
       </c>
@@ -17439,9 +17439,9 @@
     </row>
     <row r="17" spans="1:28" ht="49.5" customHeight="1">
       <c r="A17" s="24"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
       <c r="E17" s="49" t="s">
         <v>150</v>
       </c>
@@ -17473,13 +17473,13 @@
     </row>
     <row r="18" spans="1:28" ht="49.5" customHeight="1">
       <c r="A18" s="24"/>
-      <c r="B18" s="94">
+      <c r="B18" s="81">
         <v>3</v>
       </c>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="87" t="s">
         <v>153</v>
       </c>
       <c r="E18" s="49" t="s">
@@ -17513,9 +17513,9 @@
     </row>
     <row r="19" spans="1:28" ht="49.5" customHeight="1">
       <c r="A19" s="24"/>
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="81"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="56" t="s">
         <v>156</v>
       </c>
@@ -17547,8 +17547,8 @@
     </row>
     <row r="20" spans="1:28" ht="49.5" customHeight="1">
       <c r="A20" s="24"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="82"/>
       <c r="D20" s="85" t="s">
         <v>158</v>
       </c>
@@ -17583,9 +17583,9 @@
     </row>
     <row r="21" spans="1:28" ht="49.5" customHeight="1">
       <c r="A21" s="24"/>
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="49" t="s">
         <v>161</v>
       </c>
@@ -17617,9 +17617,9 @@
     </row>
     <row r="22" spans="1:28" ht="49.5" customHeight="1">
       <c r="A22" s="24"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="49" t="s">
         <v>163</v>
       </c>
@@ -17651,9 +17651,9 @@
     </row>
     <row r="23" spans="1:28" ht="49.5" customHeight="1">
       <c r="A23" s="24"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
       <c r="E23" s="49" t="s">
         <v>165</v>
       </c>
@@ -17685,13 +17685,13 @@
     </row>
     <row r="24" spans="1:28" ht="49.5" customHeight="1">
       <c r="A24" s="24"/>
-      <c r="B24" s="94">
+      <c r="B24" s="81">
         <v>4</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="84" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="93" t="s">
+      <c r="D24" s="87" t="s">
         <v>168</v>
       </c>
       <c r="E24" s="49" t="s">
@@ -17725,9 +17725,9 @@
     </row>
     <row r="25" spans="1:28" ht="49.5" customHeight="1">
       <c r="A25" s="24"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
       <c r="E25" s="49" t="s">
         <v>171</v>
       </c>
@@ -17759,13 +17759,13 @@
     </row>
     <row r="26" spans="1:28" ht="49.5" customHeight="1">
       <c r="A26" s="24"/>
-      <c r="B26" s="80">
+      <c r="B26" s="88">
         <v>5</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="93" t="s">
+      <c r="D26" s="87" t="s">
         <v>174</v>
       </c>
       <c r="E26" s="49" t="s">
@@ -17799,9 +17799,9 @@
     </row>
     <row r="27" spans="1:28" ht="49.5" customHeight="1">
       <c r="A27" s="24"/>
-      <c r="B27" s="83"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="83"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="49" t="s">
         <v>177</v>
       </c>
@@ -17833,9 +17833,9 @@
     </row>
     <row r="28" spans="1:28" ht="49.5" customHeight="1">
       <c r="A28" s="24"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="49" t="s">
         <v>179</v>
       </c>
@@ -17867,9 +17867,9 @@
     </row>
     <row r="29" spans="1:28" ht="49.5" customHeight="1">
       <c r="A29" s="24"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="81"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="83"/>
       <c r="E29" s="49" t="s">
         <v>181</v>
       </c>
@@ -17901,9 +17901,9 @@
     </row>
     <row r="30" spans="1:28" ht="49.5" customHeight="1">
       <c r="A30" s="24"/>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="93" t="s">
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="87" t="s">
         <v>183</v>
       </c>
       <c r="E30" s="49" t="s">
@@ -17937,9 +17937,9 @@
     </row>
     <row r="31" spans="1:28" ht="49.5" customHeight="1">
       <c r="A31" s="24"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
       <c r="E31" s="49" t="s">
         <v>186</v>
       </c>
@@ -17971,9 +17971,9 @@
     </row>
     <row r="32" spans="1:28" ht="49.5" customHeight="1">
       <c r="A32" s="24"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="81"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
       <c r="E32" s="49" t="s">
         <v>188</v>
       </c>
@@ -18005,13 +18005,13 @@
     </row>
     <row r="33" spans="1:28" ht="49.5" customHeight="1">
       <c r="A33" s="24"/>
-      <c r="B33" s="80">
+      <c r="B33" s="88">
         <v>6</v>
       </c>
-      <c r="C33" s="92" t="s">
+      <c r="C33" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="D33" s="93" t="s">
+      <c r="D33" s="87" t="s">
         <v>191</v>
       </c>
       <c r="E33" s="49" t="s">
@@ -18045,9 +18045,9 @@
     </row>
     <row r="34" spans="1:28" ht="49.5" customHeight="1">
       <c r="A34" s="24"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
       <c r="E34" s="58" t="s">
         <v>194</v>
       </c>
@@ -18078,36 +18078,36 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A35" s="82"/>
-      <c r="B35" s="82" t="s">
+      <c r="A35" s="91"/>
+      <c r="B35" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="C35" s="84" t="s">
+      <c r="C35" s="92" t="s">
         <v>197</v>
       </c>
       <c r="D35" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="E35" s="86" t="s">
+      <c r="E35" s="93" t="s">
         <v>199</v>
       </c>
-      <c r="F35" s="87" t="s">
+      <c r="F35" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="G35" s="88" t="s">
+      <c r="G35" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="89" t="s">
+      <c r="H35" s="96" t="s">
         <v>202</v>
       </c>
-      <c r="I35" s="90">
+      <c r="I35" s="97">
         <v>45389</v>
       </c>
-      <c r="J35" s="91" t="s">
+      <c r="J35" s="98" t="s">
         <v>203</v>
       </c>
-      <c r="K35" s="89"/>
-      <c r="L35" s="78"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="89"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
       <c r="O35" s="15"/>
@@ -18126,18 +18126,18 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A36" s="83"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="79"/>
+      <c r="A36" s="82"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="90"/>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
       <c r="O36" s="15"/>
@@ -18156,18 +18156,18 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A37" s="83"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="83"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="79"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="90"/>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
@@ -18186,18 +18186,18 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A38" s="83"/>
-      <c r="B38" s="83"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="83"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="83"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="79"/>
+      <c r="A38" s="82"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="90"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -18216,18 +18216,18 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A39" s="83"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
-      <c r="J39" s="83"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="79"/>
+      <c r="A39" s="82"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="90"/>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
@@ -18246,18 +18246,18 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A40" s="81"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="79"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="83"/>
+      <c r="J40" s="83"/>
+      <c r="K40" s="83"/>
+      <c r="L40" s="90"/>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
       <c r="O40" s="15"/>
@@ -24892,27 +24892,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="C26:C32"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
     <mergeCell ref="L35:L40"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A35:A40"/>
@@ -24926,6 +24905,27 @@
     <mergeCell ref="I35:I40"/>
     <mergeCell ref="J35:J40"/>
     <mergeCell ref="K35:K40"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:C32"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="B10:B17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -31705,7 +31705,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31807,7 +31807,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>18</v>
+        <v>18.5</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32093,7 +32093,7 @@
         <v>231</v>
       </c>
       <c r="D11" s="7">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>

</xml_diff>

<commit_message>
Completed LO 5-3 summarize at least two tangible examples of how they changed the culture of their team or organization
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BB2D41-F431-CD46-9D0F-9CF1CFEEE4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E7344-9776-C842-AA02-89E5C6A0CE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="235">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -1722,10 +1722,16 @@
     <t>Deep dive L0 3.5 -3.6</t>
   </si>
   <si>
-    <t>Deep dive - LO 4.1</t>
+    <t>4/18/24</t>
   </si>
   <si>
-    <t>4/18/24</t>
+    <t>4/19/24</t>
+  </si>
+  <si>
+    <t>Deep dive - 5.3</t>
+  </si>
+  <si>
+    <t>Deep dive - LO 4.1 - L0 5.2</t>
   </si>
 </sst>
 </file>
@@ -31705,7 +31711,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31807,7 +31813,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32084,16 +32090,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B11" s="77" t="s">
         <v>219</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D11" s="7">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -32119,10 +32125,18 @@
       <c r="Z11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>

</xml_diff>

<commit_message>
Completed LO 5-6 – Experiment with at least three techniques to improve inter-team collaboration
</commit_message>
<xml_diff>
--- a/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
+++ b/02 - CSP-SM Mentee Mapping Learning Log - ED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/esuabomdijemeni/Desktop/github/csp-sm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0E7344-9776-C842-AA02-89E5C6A0CE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604D43C2-B12C-7F44-B8FC-054713872E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="237">
   <si>
     <t>A note about Bloom's Taxonomy</t>
   </si>
@@ -1733,6 +1733,12 @@
   <si>
     <t>Deep dive - LO 4.1 - L0 5.2</t>
   </si>
+  <si>
+    <t>Deep dive - 5.5-5.6</t>
+  </si>
+  <si>
+    <t>4/20/24</t>
+  </si>
 </sst>
 </file>
 
@@ -31711,7 +31717,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -31813,7 +31819,7 @@
       <c r="E3" s="15"/>
       <c r="F3" s="70">
         <f>SUM(D2:D1048576)</f>
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -32161,10 +32167,18 @@
       <c r="Z12" s="15"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>

</xml_diff>